<commit_message>
Pages and other files
</commit_message>
<xml_diff>
--- a/src/main/resources/ExcelFiles/ManageDeliveryBoyData.xlsx
+++ b/src/main/resources/ExcelFiles/ManageDeliveryBoyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ajal\Java\Eclipse\com.sevenrmartsupermarket\src\main\resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8B60F2-33BE-4C1F-AAF7-A00BBB443C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8118B8E-7692-478A-971A-778D096EC1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13032" yWindow="180" windowWidth="10008" windowHeight="10344" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="10008" windowHeight="10344" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Delivery Boy Details" sheetId="1" r:id="rId1"/>
@@ -27,19 +27,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Don</t>
+    <t>Mark</t>
   </si>
   <si>
-    <t>don@gmail.com</t>
+    <t>mark@gmail.com</t>
   </si>
   <si>
-    <t>don458</t>
+    <t>Kerala</t>
   </si>
   <si>
-    <t>Erode</t>
+    <t>merk66</t>
   </si>
   <si>
-    <t>D_O_N007</t>
+    <t>mark</t>
   </si>
 </sst>
 </file>
@@ -371,7 +371,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -391,22 +391,22 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>9895615595</v>
+        <v>9835615595</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>